<commit_message>
Created code for KK phase retrieveal
</commit_message>
<xml_diff>
--- a/interferometry/data/metadata.xlsx
+++ b/interferometry/data/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfc365-my.sharepoint.com/personal/jamie_watts_stfc_ac_uk/Documents/Documents/python/interferometry/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfc365-my.sharepoint.com/personal/jamie_watts_stfc_ac_uk/Documents/Documents/python/git_projects/THz-interferometry/interferometry/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="5" documentId="8_{B7647863-2C0E-490F-8303-FF2D4490FB04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9C8F441-8070-4ECE-A884-DE1A7FED25D3}"/>
   <bookViews>
-    <workbookView xWindow="4125" yWindow="1680" windowWidth="21600" windowHeight="11385" xr2:uid="{4B806992-E72D-4EE1-A88B-5E65FA320BF8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4B806992-E72D-4EE1-A88B-5E65FA320BF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -325,10 +325,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -651,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB241B61-43AC-4CD0-8506-51CD40367140}">
   <dimension ref="A1:I76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="F77" sqref="F77"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>